<commit_message>
update to rev 2
</commit_message>
<xml_diff>
--- a/LED_switch_pairs.xlsx
+++ b/LED_switch_pairs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\Muse\694210101R1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\Muse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C67380-7601-4EA8-876B-5CAD833FD9B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7813474-F0A4-4DC3-A465-A217DBE693CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7978CB14-2F27-4BCB-813E-6B983813FA6D}"/>
+    <workbookView xWindow="2220" yWindow="576" windowWidth="20676" windowHeight="11256" xr2:uid="{7978CB14-2F27-4BCB-813E-6B983813FA6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,13 +84,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,13 +114,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,20 +436,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E141B0AC-BBD2-4D99-B106-AE7919EB216F}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +514,7 @@
         <v>D169</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -549,7 +564,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -614,7 +629,7 @@
         <v>D170</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -664,7 +679,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -729,7 +744,7 @@
         <v>D171</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -778,8 +793,12 @@
       <c r="P7">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T7">
+        <f>4*16</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -839,12 +858,12 @@
         <f t="shared" si="12"/>
         <v>D168</v>
       </c>
-      <c r="P8" t="str">
+      <c r="P8" s="1" t="str">
         <f t="shared" ref="P8" si="13">"D"&amp;(VALUE(RIGHT(O8,3))+4)</f>
         <v>D172</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -890,16 +909,16 @@
       <c r="O9">
         <v>86</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -948,7 +967,7 @@
         <v>D217</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -985,8 +1004,12 @@
       <c r="L14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T14">
+        <f>4*12</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1030,12 +1053,16 @@
         <f t="shared" si="15"/>
         <v>D214</v>
       </c>
-      <c r="L15" t="str">
+      <c r="L15" s="1" t="str">
         <f t="shared" si="15"/>
         <v>D218</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T15">
+        <f>T14+T7</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1069,7 +1096,7 @@
       <c r="K16">
         <v>83</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1">
         <v>87</v>
       </c>
     </row>
@@ -1192,7 +1219,7 @@
         <f t="shared" si="17"/>
         <v>D204</v>
       </c>
-      <c r="I19" t="str">
+      <c r="I19" s="1" t="str">
         <f t="shared" si="17"/>
         <v>D208</v>
       </c>
@@ -1234,7 +1261,7 @@
       <c r="H20">
         <v>105</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J20" t="s">

</xml_diff>